<commit_message>
updated dyson and dba excel
</commit_message>
<xml_diff>
--- a/dba_BA.xlsx
+++ b/dba_BA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauro/Desktop/THESIS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauro/Desktop/TCCM_Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D4D4DC-6090-E746-8645-F4E65E1BA2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2512F23-7736-DF40-A709-69CC73A4D2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1300" windowWidth="27220" windowHeight="15440" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
+    <workbookView xWindow="2140" yWindow="1300" windowWidth="27220" windowHeight="15440" activeTab="5" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="dba_all" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="quinones_S2018" sheetId="4" r:id="rId3"/>
     <sheet name="He12" sheetId="5" r:id="rId4"/>
     <sheet name="H2O" sheetId="6" r:id="rId5"/>
+    <sheet name="Q0_Q1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="118">
   <si>
     <t>2s1p</t>
   </si>
@@ -350,6 +351,72 @@
   </si>
   <si>
     <t>BSSE E H2O</t>
+  </si>
+  <si>
+    <t>Q0_181_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_262_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_329_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_349_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_360_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_6_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_73_dba.out</t>
+  </si>
+  <si>
+    <t>Q0_90_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_115_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_151_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_181_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_229_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_249_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_289_dba.out</t>
+  </si>
+  <si>
+    <t>Q1_73_dba.out</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Dih1</t>
+  </si>
+  <si>
+    <t>Dih2</t>
+  </si>
+  <si>
+    <t>dba (meV)</t>
+  </si>
+  <si>
+    <t>vba (eV)</t>
   </si>
 </sst>
 </file>
@@ -720,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -895,6 +962,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7493,7 +7569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E42B7A-694B-1242-8C9E-27563F12182D}">
   <dimension ref="B2:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" workbookViewId="0">
+    <sheetView topLeftCell="D32" workbookViewId="0">
       <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
@@ -12729,4 +12805,402 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1E6734-98D3-D44C-BC8D-6181C969C7A5}">
+  <dimension ref="B1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C1" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="24">
+        <v>-172.63</v>
+      </c>
+      <c r="E2" s="24">
+        <v>-154.41999999999999</v>
+      </c>
+      <c r="F2" s="82">
+        <v>-12.320819999999999</v>
+      </c>
+      <c r="G2" s="83">
+        <v>1.5359989999999999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="24">
+        <v>-101.95</v>
+      </c>
+      <c r="E3" s="24">
+        <v>-64.349999999999994</v>
+      </c>
+      <c r="F3" s="82">
+        <v>7.9304800000000002</v>
+      </c>
+      <c r="G3" s="83">
+        <v>-1.94320648</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="81" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="24">
+        <v>-25.74</v>
+      </c>
+      <c r="E4" s="24">
+        <v>123.84</v>
+      </c>
+      <c r="F4" s="82">
+        <v>-6.9801000000000002</v>
+      </c>
+      <c r="G4" s="83">
+        <v>-1.8649961399999999</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="24">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E5" s="24">
+        <v>143.16</v>
+      </c>
+      <c r="F5" s="82">
+        <v>-2.8273899999999998</v>
+      </c>
+      <c r="G5" s="83">
+        <v>-1.7934479999999999</v>
+      </c>
+      <c r="H5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C6" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="24">
+        <v>-0.09</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="82">
+        <v>7.9555499999999997</v>
+      </c>
+      <c r="G6" s="83">
+        <v>-1.8505689700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="24">
+        <v>-0.48</v>
+      </c>
+      <c r="E7" s="24">
+        <v>123.8</v>
+      </c>
+      <c r="F7" s="82">
+        <v>-3.5990199999999999</v>
+      </c>
+      <c r="G7" s="83">
+        <v>-1.8543510000000001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="81" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="24">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="E8" s="24">
+        <v>-44.37</v>
+      </c>
+      <c r="F8" s="82">
+        <v>-1.94164</v>
+      </c>
+      <c r="G8" s="83">
+        <v>-1.955392</v>
+      </c>
+      <c r="H8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C9" s="81" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="24">
+        <v>81.89</v>
+      </c>
+      <c r="E9" s="24">
+        <v>-81.52</v>
+      </c>
+      <c r="F9" s="82">
+        <v>-4.7393799999999997</v>
+      </c>
+      <c r="G9" s="83">
+        <v>-1.9617100000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="83"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="24">
+        <v>123.82</v>
+      </c>
+      <c r="E11" s="24">
+        <v>3.57</v>
+      </c>
+      <c r="F11" s="82">
+        <v>-4.04646E-3</v>
+      </c>
+      <c r="G11" s="83">
+        <v>-1.293175</v>
+      </c>
+      <c r="H11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="24">
+        <v>142.5</v>
+      </c>
+      <c r="E12" s="24">
+        <v>-23.71</v>
+      </c>
+      <c r="F12" s="82">
+        <v>-4.4179900000000001E-3</v>
+      </c>
+      <c r="G12" s="83">
+        <v>-1.2638959999999999</v>
+      </c>
+      <c r="H12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="81" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="24">
+        <v>178.71</v>
+      </c>
+      <c r="E13" s="24">
+        <v>-178.52</v>
+      </c>
+      <c r="F13" s="82">
+        <v>-1.390486E-2</v>
+      </c>
+      <c r="G13" s="83">
+        <v>-0.93933999999999995</v>
+      </c>
+      <c r="H13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="24">
+        <v>-123.62</v>
+      </c>
+      <c r="E14" s="24">
+        <v>3.91</v>
+      </c>
+      <c r="F14" s="82">
+        <v>-7.8382199999999999E-3</v>
+      </c>
+      <c r="G14" s="83">
+        <v>-1.3071459999999999</v>
+      </c>
+      <c r="H14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="81" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="24">
+        <v>-101.97</v>
+      </c>
+      <c r="E15" s="24">
+        <v>27.29</v>
+      </c>
+      <c r="F15" s="82">
+        <v>-1.109392E-2</v>
+      </c>
+      <c r="G15" s="83">
+        <v>-1.354036</v>
+      </c>
+      <c r="H15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="24">
+        <v>-65.52</v>
+      </c>
+      <c r="E16" s="24">
+        <v>65.98</v>
+      </c>
+      <c r="F16" s="82">
+        <v>-1.0271840000000001E-2</v>
+      </c>
+      <c r="G16" s="83">
+        <v>-1.4243969999999999</v>
+      </c>
+      <c r="H16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="24">
+        <v>64.42</v>
+      </c>
+      <c r="E17" s="24">
+        <v>-64.319999999999993</v>
+      </c>
+      <c r="F17" s="82">
+        <v>-5.4201400000000004E-3</v>
+      </c>
+      <c r="G17" s="83">
+        <v>-1.4336679999999999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="G22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+      <c r="G23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="G24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+      <c r="G25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="G26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Included Dyson-cc2 equation. Still need to be revised
</commit_message>
<xml_diff>
--- a/dba_BA.xlsx
+++ b/dba_BA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauro/Desktop/TCCM_Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2512F23-7736-DF40-A709-69CC73A4D2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2835196-661A-2841-923C-C603F8B88E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="1300" windowWidth="27220" windowHeight="15440" activeTab="5" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="124">
   <si>
     <t>2s1p</t>
   </si>
@@ -417,6 +417,24 @@
   </si>
   <si>
     <t>vba (eV)</t>
+  </si>
+  <si>
+    <t>Qa_265I_EA.in</t>
+  </si>
+  <si>
+    <t>Qa_265N_EA.in</t>
+  </si>
+  <si>
+    <t>Qa_265S_EA.in</t>
+  </si>
+  <si>
+    <t>Qa_265T_EA.in</t>
+  </si>
+  <si>
+    <t>Qa_EA.in</t>
+  </si>
+  <si>
+    <t>Quinone + aa</t>
   </si>
 </sst>
 </file>
@@ -924,6 +942,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -962,15 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7587,36 +7605,36 @@
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B2" s="11"/>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="75" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
     </row>
     <row r="3" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="75" t="s">
+      <c r="D3" s="80"/>
+      <c r="E3" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76" t="s">
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="76"/>
-      <c r="K3" s="73" t="s">
+      <c r="J3" s="79"/>
+      <c r="K3" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="74"/>
+      <c r="L3" s="77"/>
       <c r="O3" s="8" t="s">
         <v>22</v>
       </c>
@@ -8693,11 +8711,11 @@
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
       <c r="J23" s="39"/>
-      <c r="K23" s="68" t="s">
+      <c r="K23" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="L23" s="68"/>
-      <c r="M23" s="69"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="72"/>
       <c r="N23" s="16" t="s">
         <v>57</v>
       </c>
@@ -9175,11 +9193,11 @@
       </c>
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="F39" s="70" t="s">
+      <c r="F39" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="G39" s="71"/>
-      <c r="H39" s="72"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="75"/>
       <c r="J39" s="13" t="s">
         <v>78</v>
       </c>
@@ -10842,14 +10860,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="78" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="79"/>
+      <c r="E1" s="82"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="50" t="s">
@@ -11610,11 +11628,11 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L14" s="60"/>
-      <c r="N14" s="76" t="s">
+      <c r="N14" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
       <c r="Y14" s="64"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -12809,10 +12827,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1E6734-98D3-D44C-BC8D-6181C969C7A5}">
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12822,7 +12840,7 @@
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C1" s="44" t="s">
         <v>113</v>
       </c>
@@ -12839,8 +12857,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="81" t="s">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C2" s="68" t="s">
         <v>96</v>
       </c>
       <c r="D2" s="24">
@@ -12849,18 +12867,18 @@
       <c r="E2" s="24">
         <v>-154.41999999999999</v>
       </c>
-      <c r="F2" s="82">
+      <c r="F2" s="69">
         <v>-12.320819999999999</v>
       </c>
-      <c r="G2" s="83">
+      <c r="G2" s="70">
         <v>1.5359989999999999</v>
       </c>
       <c r="H2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="81" t="s">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C3" s="68" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="24">
@@ -12869,15 +12887,15 @@
       <c r="E3" s="24">
         <v>-64.349999999999994</v>
       </c>
-      <c r="F3" s="82">
+      <c r="F3" s="69">
         <v>7.9304800000000002</v>
       </c>
-      <c r="G3" s="83">
+      <c r="G3" s="70">
         <v>-1.94320648</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="81" t="s">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C4" s="68" t="s">
         <v>98</v>
       </c>
       <c r="D4" s="24">
@@ -12886,15 +12904,15 @@
       <c r="E4" s="24">
         <v>123.84</v>
       </c>
-      <c r="F4" s="82">
+      <c r="F4" s="69">
         <v>-6.9801000000000002</v>
       </c>
-      <c r="G4" s="83">
+      <c r="G4" s="70">
         <v>-1.8649961399999999</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="81" t="s">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C5" s="68" t="s">
         <v>99</v>
       </c>
       <c r="D5" s="24">
@@ -12903,18 +12921,18 @@
       <c r="E5" s="24">
         <v>143.16</v>
       </c>
-      <c r="F5" s="82">
+      <c r="F5" s="69">
         <v>-2.8273899999999998</v>
       </c>
-      <c r="G5" s="83">
+      <c r="G5" s="70">
         <v>-1.7934479999999999</v>
       </c>
       <c r="H5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="81" t="s">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C6" s="68" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="24">
@@ -12923,15 +12941,15 @@
       <c r="E6" s="24">
         <v>0.05</v>
       </c>
-      <c r="F6" s="82">
+      <c r="F6" s="69">
         <v>7.9555499999999997</v>
       </c>
-      <c r="G6" s="83">
+      <c r="G6" s="70">
         <v>-1.8505689700000001</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="81" t="s">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C7" s="68" t="s">
         <v>101</v>
       </c>
       <c r="D7" s="24">
@@ -12940,18 +12958,18 @@
       <c r="E7" s="24">
         <v>123.8</v>
       </c>
-      <c r="F7" s="82">
+      <c r="F7" s="69">
         <v>-3.5990199999999999</v>
       </c>
-      <c r="G7" s="83">
+      <c r="G7" s="70">
         <v>-1.8543510000000001</v>
       </c>
       <c r="H7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="81" t="s">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C8" s="68" t="s">
         <v>102</v>
       </c>
       <c r="D8" s="24">
@@ -12960,18 +12978,18 @@
       <c r="E8" s="24">
         <v>-44.37</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="69">
         <v>-1.94164</v>
       </c>
-      <c r="G8" s="83">
+      <c r="G8" s="70">
         <v>-1.955392</v>
       </c>
       <c r="H8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="81" t="s">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C9" s="68" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="24">
@@ -12980,25 +12998,27 @@
       <c r="E9" s="24">
         <v>-81.52</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="69">
         <v>-4.7393799999999997</v>
       </c>
-      <c r="G9" s="83">
+      <c r="G9" s="70">
         <v>-1.9617100000000001</v>
       </c>
       <c r="H9" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="83"/>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="81" t="s">
+      <c r="F10" s="69"/>
+      <c r="G10" s="70"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C11" s="68" t="s">
         <v>104</v>
       </c>
       <c r="D11" s="24">
@@ -13007,18 +13027,19 @@
       <c r="E11" s="24">
         <v>3.57</v>
       </c>
-      <c r="F11" s="82">
-        <v>-4.04646E-3</v>
-      </c>
-      <c r="G11" s="83">
+      <c r="F11" s="69">
+        <v>-4.0464599999999997</v>
+      </c>
+      <c r="G11" s="70">
         <v>-1.293175</v>
       </c>
       <c r="H11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="81" t="s">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C12" s="68" t="s">
         <v>105</v>
       </c>
       <c r="D12" s="24">
@@ -13027,18 +13048,19 @@
       <c r="E12" s="24">
         <v>-23.71</v>
       </c>
-      <c r="F12" s="82">
-        <v>-4.4179900000000001E-3</v>
-      </c>
-      <c r="G12" s="83">
+      <c r="F12" s="69">
+        <v>-4.4179899999999996</v>
+      </c>
+      <c r="G12" s="70">
         <v>-1.2638959999999999</v>
       </c>
       <c r="H12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="81" t="s">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C13" s="68" t="s">
         <v>106</v>
       </c>
       <c r="D13" s="24">
@@ -13047,18 +13069,19 @@
       <c r="E13" s="24">
         <v>-178.52</v>
       </c>
-      <c r="F13" s="82">
-        <v>-1.390486E-2</v>
-      </c>
-      <c r="G13" s="83">
+      <c r="F13" s="69">
+        <v>-13.904859999999999</v>
+      </c>
+      <c r="G13" s="70">
         <v>-0.93933999999999995</v>
       </c>
       <c r="H13" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="81" t="s">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C14" s="68" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="24">
@@ -13067,18 +13090,18 @@
       <c r="E14" s="24">
         <v>3.91</v>
       </c>
-      <c r="F14" s="82">
-        <v>-7.8382199999999999E-3</v>
-      </c>
-      <c r="G14" s="83">
+      <c r="F14" s="69">
+        <v>-7.8382199999999997</v>
+      </c>
+      <c r="G14" s="70">
         <v>-1.3071459999999999</v>
       </c>
       <c r="H14" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="81" t="s">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C15" s="68" t="s">
         <v>108</v>
       </c>
       <c r="D15" s="24">
@@ -13087,18 +13110,18 @@
       <c r="E15" s="24">
         <v>27.29</v>
       </c>
-      <c r="F15" s="82">
-        <v>-1.109392E-2</v>
-      </c>
-      <c r="G15" s="83">
+      <c r="F15" s="69">
+        <v>-11.093920000000001</v>
+      </c>
+      <c r="G15" s="70">
         <v>-1.354036</v>
       </c>
       <c r="H15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C16" s="81" t="s">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C16" s="68" t="s">
         <v>109</v>
       </c>
       <c r="D16" s="24">
@@ -13107,18 +13130,18 @@
       <c r="E16" s="24">
         <v>65.98</v>
       </c>
-      <c r="F16" s="82">
-        <v>-1.0271840000000001E-2</v>
-      </c>
-      <c r="G16" s="83">
+      <c r="F16" s="69">
+        <v>-10.271839999999999</v>
+      </c>
+      <c r="G16" s="70">
         <v>-1.4243969999999999</v>
       </c>
       <c r="H16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="81" t="s">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="68" t="s">
         <v>110</v>
       </c>
       <c r="D17" s="24">
@@ -13127,68 +13150,121 @@
       <c r="E17" s="24">
         <v>-64.319999999999993</v>
       </c>
-      <c r="F17" s="82">
-        <v>-5.4201400000000004E-3</v>
-      </c>
-      <c r="G17" s="83">
+      <c r="F17" s="69">
+        <v>-5.42014</v>
+      </c>
+      <c r="G17" s="70">
         <v>-1.4336679999999999</v>
       </c>
       <c r="H17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21">
+        <v>-78.069999999999993</v>
+      </c>
+      <c r="E21">
+        <v>114.06</v>
+      </c>
       <c r="G21" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22">
+        <v>-76.260000000000005</v>
+      </c>
+      <c r="E22">
+        <v>135.44999999999999</v>
+      </c>
       <c r="G22" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
+        <v>-81.78</v>
+      </c>
+      <c r="E23">
+        <v>126.05</v>
+      </c>
       <c r="G23" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24">
+        <v>-83.54</v>
+      </c>
+      <c r="E24">
+        <v>118.17</v>
+      </c>
       <c r="G24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25">
+        <v>-78.069999999999993</v>
+      </c>
+      <c r="E25">
+        <v>112.31</v>
+      </c>
       <c r="G25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="G26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added gnuplot plots and small changes
</commit_message>
<xml_diff>
--- a/dba_BA.xlsx
+++ b/dba_BA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauro/Desktop/TCCM_Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA62A9D-11F3-7F47-B894-A6AB7C75EB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850ADAD2-8F02-0B40-8457-D362CFEE6F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1300" windowWidth="27220" windowHeight="15440" activeTab="4" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
+    <workbookView xWindow="2140" yWindow="1280" windowWidth="27220" windowHeight="15440" activeTab="4" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="dba_all" sheetId="2" r:id="rId1"/>
@@ -808,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -993,7 +993,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8311,16 +8310,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>694267</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>186267</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180559</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>406556</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>65067</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>720488</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>79337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8347,16 +8346,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371592</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>149263</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414401</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177802</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>188148</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>78394</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>230958</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>106933</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12274,8 +12273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FBACF4-8C00-9C4D-8432-3950F06E07EB}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="118" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A12" zoomScale="118" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13357,10 +13356,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF798BE4-C0A1-7940-9885-95EEF6FDCBCD}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13470,7 +13469,7 @@
       <c r="Q3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="R3" s="84" t="s">
+      <c r="R3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -13590,7 +13589,7 @@
         <v>115.24284606207256</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5:R13" si="6">(L5-J5)*27211.407953</f>
+        <f t="shared" ref="R5:R12" si="6">(L5-J5)*27211.407953</f>
         <v>-4.0408532618718986</v>
       </c>
     </row>
@@ -13974,12 +13973,196 @@
         <v>-12.235639521281396</v>
       </c>
       <c r="R13">
-        <f t="shared" si="6"/>
+        <f>(L13-J13)*27211.407953</f>
         <v>-12.340855150407286</v>
       </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <f>(J4-J$13)*27211.407953</f>
+        <v>114473.92294368258</v>
+      </c>
+      <c r="K15">
+        <f>(K4-$J4)*27211.407953</f>
+        <v>-868.12198595148936</v>
+      </c>
+      <c r="L15">
+        <f>(L4-$J4)*27211.407953</f>
+        <v>-44.570961032540204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <f>(J5-J$13)*27211.407953</f>
+        <v>-9.7345138429135361</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:L16" si="7">(K5-$J5)*27211.407953</f>
+        <v>-2247.7368643387367</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="7"/>
+        <v>-4.0408532618718986</v>
+      </c>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <f>(J6-J$13)*27211.407953</f>
+        <v>-54.091655792522843</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17:L17" si="8">(K6-$J6)*27211.407953</f>
+        <v>-1885.595008967693</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="8"/>
+        <v>-39.719439108381621</v>
+      </c>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <f>(J7-J$13)*27211.407953</f>
+        <v>-5.6998430087997276</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:L18" si="9">(K7-$J7)*27211.407953</f>
+        <v>-1803.6648746535084</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="9"/>
+        <v>-58.445706922394606</v>
+      </c>
+    </row>
+    <row r="19" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <f>(J8-J$13)*27211.407953</f>
+        <v>2.8188295142117344E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ref="K19:L19" si="10">(K8-$J8)*27211.407953</f>
+        <v>-1767.3356640433403</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="10"/>
+        <v>-57.671841686850712</v>
+      </c>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>12</v>
+      </c>
+      <c r="J20">
+        <f>(J9-J$13)*27211.407953</f>
+        <v>0.78183817109653242</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ref="K20:L20" si="11">(K9-$J9)*27211.407953</f>
+        <v>-1747.7720277381154</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="11"/>
+        <v>-51.153890419404654</v>
+      </c>
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>15</v>
+      </c>
+      <c r="J21">
+        <f>(J10-J$13)*27211.407953</f>
+        <v>0.66324813409682515</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:L21" si="12">(K10-$J10)*27211.407953</f>
+        <v>-1731.8827369631331</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="12"/>
+        <v>-41.080442164357123</v>
+      </c>
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>20</v>
+      </c>
+      <c r="J22">
+        <f>(J11-J$13)*27211.407953</f>
+        <v>0.20742439853594022</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:L22" si="13">(K11-$J11)*27211.407953</f>
+        <v>-1719.6398537680323</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="13"/>
+        <v>-29.280340281271553</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>30</v>
+      </c>
+      <c r="J23">
+        <f>(J12-J$13)*27211.407953</f>
+        <v>6.9563242666231234E-2</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="K23:L23" si="14">(K12-$J12)*27211.407953</f>
+        <v>-1711.0149667209166</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="14"/>
+        <v>-17.568942142633045</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>40</v>
+      </c>
+      <c r="J24">
+        <f>(J13-J$13)*27211.407953</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>(K13-$J13)*27.211407953</f>
+        <v>-1.7080320195286753</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="K24:L24" si="15">(L13-$J13)*27211.407953</f>
+        <v>-12.340855150407286</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+    </row>
+    <row r="26" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+    </row>
+    <row r="27" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added figure in results
</commit_message>
<xml_diff>
--- a/dba_BA.xlsx
+++ b/dba_BA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauro/Desktop/TCCM_Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850ADAD2-8F02-0B40-8457-D362CFEE6F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9AC8A-E607-B045-AFAD-08EDCCF76541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1280" windowWidth="27220" windowHeight="15440" activeTab="4" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
+    <workbookView xWindow="3980" yWindow="1260" windowWidth="25380" windowHeight="15440" activeTab="2" xr2:uid="{DAC46931-DB7F-0643-9A3F-CDCD008B5FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="dba_all" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="157">
   <si>
     <t>2s1p</t>
   </si>
@@ -439,6 +439,560 @@
   <si>
     <t>dba - BSSE</t>
   </si>
+  <si>
+    <t>ri-CC2 aug-cc-pVTZ</t>
+  </si>
+  <si>
+    <t>KT</t>
+  </si>
+  <si>
+    <t>μ (D)</t>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NO </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>SO </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>NCHO </t>
+    </r>
+  </si>
+  <si>
+    <t>N,N-Dimethylformamide</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>CHO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>CN </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>CO</t>
+    </r>
+  </si>
+  <si>
+    <t>CH3CHO</t>
+  </si>
+  <si>
+    <t>Acetaldehyde</t>
+  </si>
+  <si>
+    <t>Acetone</t>
+  </si>
+  <si>
+    <t>Acetonitrile</t>
+  </si>
+  <si>
+    <t>Benzaldehyde</t>
+  </si>
+  <si>
+    <t>DMSO</t>
+  </si>
+  <si>
+    <t>Formamide</t>
+  </si>
+  <si>
+    <t>Methylisocyanide</t>
+  </si>
+  <si>
+    <t>Nitrobenzene</t>
+  </si>
+  <si>
+    <t>Nitromethane</t>
+  </si>
+  <si>
+    <t>Nitrosobenzene</t>
+  </si>
+  <si>
+    <t>Phenylisocyanide</t>
+  </si>
+  <si>
+    <t>Pyridazine</t>
+  </si>
+  <si>
+    <t>Vinylene carbonate</t>
+  </si>
+  <si>
+    <t>Molecule</t>
+  </si>
 </sst>
 </file>
 
@@ -448,7 +1002,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -513,6 +1067,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -808,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -954,12 +1514,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,6 +1540,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -991,6 +1553,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1310,8 +1875,38 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -8700,10 +9295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E42B7A-694B-1242-8C9E-27563F12182D}">
-  <dimension ref="B2:Y55"/>
+  <dimension ref="B2:AG55"/>
   <sheetViews>
-    <sheetView topLeftCell="D32" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView topLeftCell="Q24" workbookViewId="0">
+      <selection activeCell="AE55" sqref="X55:AE55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9638,7 +10233,7 @@
         <v>4.3232600000000012</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
         <v>15</v>
       </c>
@@ -9706,7 +10301,7 @@
         <v>0.36436999999999997</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>38</v>
       </c>
@@ -9765,7 +10360,7 @@
         <v>0.10000000000000009</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:33" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="Q19" s="1"/>
       <c r="S19" s="35"/>
       <c r="W19" s="33" t="s">
@@ -9780,7 +10375,7 @@
         <v>2.804900714285715</v>
       </c>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B20" s="40" t="s">
         <v>45</v>
       </c>
@@ -9808,10 +10403,10 @@
       <c r="X20" s="40"/>
       <c r="Y20" s="40"/>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.2">
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
@@ -9820,23 +10415,23 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.2">
       <c r="F23" s="36"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
       <c r="J23" s="39"/>
-      <c r="K23" s="71" t="s">
+      <c r="K23" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="L23" s="71"/>
-      <c r="M23" s="72"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="82"/>
       <c r="N23" s="16" t="s">
         <v>57</v>
       </c>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F24" s="45" t="s">
         <v>54</v>
       </c>
@@ -9863,7 +10458,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E25" s="13" t="s">
         <v>3</v>
       </c>
@@ -9894,8 +10489,25 @@
       <c r="O25" s="16">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="U25" s="11"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="80"/>
+      <c r="X25" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y25" s="79"/>
+      <c r="Z25" s="79"/>
+      <c r="AA25" s="79"/>
+      <c r="AB25" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC25" s="79"/>
+      <c r="AD25" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE25" s="77"/>
+    </row>
+    <row r="26" spans="2:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E26" s="13" t="s">
         <v>4</v>
       </c>
@@ -9926,8 +10538,41 @@
       <c r="O26" s="16">
         <v>-0.9</v>
       </c>
-    </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="U26" s="15"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB26" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD26" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF26" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG26" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E27" s="14" t="s">
         <v>5</v>
       </c>
@@ -9958,8 +10603,44 @@
       <c r="O27" s="16">
         <v>-18.399999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V27" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="X27" s="71">
+        <v>-156.69999999999999</v>
+      </c>
+      <c r="Y27" s="71">
+        <v>-27.8</v>
+      </c>
+      <c r="Z27" s="71">
+        <v>-3.2</v>
+      </c>
+      <c r="AA27" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="AB27" s="71">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="AC27" s="71">
+        <v>-3.2</v>
+      </c>
+      <c r="AD27" s="71">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="AE27" s="71">
+        <v>-3.1</v>
+      </c>
+      <c r="AF27">
+        <v>-0.42799999999999999</v>
+      </c>
+      <c r="AG27" s="72">
+        <v>3.2917000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E28" s="13" t="s">
         <v>6</v>
       </c>
@@ -9990,8 +10671,44 @@
       <c r="O28" s="16">
         <v>-4.5999999999999996</v>
       </c>
-    </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V28" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="X28" s="71">
+        <v>-114.9</v>
+      </c>
+      <c r="Y28" s="71">
+        <v>-16.8</v>
+      </c>
+      <c r="Z28" s="71">
+        <v>1.3</v>
+      </c>
+      <c r="AA28" s="71">
+        <v>3.3</v>
+      </c>
+      <c r="AB28" s="71">
+        <v>-0.3</v>
+      </c>
+      <c r="AC28" s="71">
+        <v>0.9</v>
+      </c>
+      <c r="AD28" s="71">
+        <v>-0.5</v>
+      </c>
+      <c r="AE28" s="71">
+        <v>0.9</v>
+      </c>
+      <c r="AF28">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="AG28" s="72">
+        <v>3.4621</v>
+      </c>
+    </row>
+    <row r="29" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E29" s="13" t="s">
         <v>7</v>
       </c>
@@ -10022,8 +10739,44 @@
       <c r="O29" s="16">
         <v>-13.7</v>
       </c>
-    </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V29" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="X29" s="71">
+        <v>-61.2</v>
+      </c>
+      <c r="Y29" s="71">
+        <v>12.6</v>
+      </c>
+      <c r="Z29" s="71">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="AA29" s="71">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="AB29" s="71">
+        <v>18.2</v>
+      </c>
+      <c r="AC29" s="71">
+        <v>20.3</v>
+      </c>
+      <c r="AD29" s="71">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AE29" s="71">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AF29">
+        <v>4.2</v>
+      </c>
+      <c r="AG29" s="72">
+        <v>4.2931999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E30" s="14" t="s">
         <v>8</v>
       </c>
@@ -10054,8 +10807,44 @@
       <c r="O30" s="16">
         <v>-14.9</v>
       </c>
-    </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V30" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="X30" s="71">
+        <v>-97.1</v>
+      </c>
+      <c r="Y30" s="71">
+        <v>-2.1</v>
+      </c>
+      <c r="Z30" s="71">
+        <v>8.9</v>
+      </c>
+      <c r="AA30" s="71">
+        <v>9.6</v>
+      </c>
+      <c r="AB30" s="71">
+        <v>7.4</v>
+      </c>
+      <c r="AC30" s="71">
+        <v>9.1</v>
+      </c>
+      <c r="AD30" s="71">
+        <v>3.4</v>
+      </c>
+      <c r="AE30" s="71">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AF30">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="AG30" s="72">
+        <v>3.7652999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E31" s="13" t="s">
         <v>9</v>
       </c>
@@ -10086,8 +10875,44 @@
       <c r="O31" s="16">
         <v>-15.9</v>
       </c>
-    </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V31" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="X31" s="71">
+        <v>-81.099999999999994</v>
+      </c>
+      <c r="Y31" s="71">
+        <v>5.4</v>
+      </c>
+      <c r="Z31" s="71">
+        <v>14.1</v>
+      </c>
+      <c r="AA31" s="71">
+        <v>14.4</v>
+      </c>
+      <c r="AB31" s="71">
+        <v>13.2</v>
+      </c>
+      <c r="AC31" s="71">
+        <v>14.4</v>
+      </c>
+      <c r="AD31" s="71">
+        <v>13.3</v>
+      </c>
+      <c r="AE31" s="71">
+        <v>13.7</v>
+      </c>
+      <c r="AF31">
+        <v>1.9</v>
+      </c>
+      <c r="AG31" s="72">
+        <v>4.4821</v>
+      </c>
+    </row>
+    <row r="32" spans="2:33" x14ac:dyDescent="0.2">
       <c r="E32" s="13" t="s">
         <v>10</v>
       </c>
@@ -10118,8 +10943,44 @@
       <c r="O32" s="16">
         <v>-9</v>
       </c>
-    </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V32" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="X32" s="71">
+        <v>-84.5</v>
+      </c>
+      <c r="Y32" s="71">
+        <v>4</v>
+      </c>
+      <c r="Z32" s="71">
+        <v>15.4</v>
+      </c>
+      <c r="AA32" s="71">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AB32" s="71">
+        <v>14.8</v>
+      </c>
+      <c r="AC32" s="71">
+        <v>15.5</v>
+      </c>
+      <c r="AD32" s="71">
+        <v>14.7</v>
+      </c>
+      <c r="AE32" s="71">
+        <v>14.9</v>
+      </c>
+      <c r="AF32">
+        <v>2.1</v>
+      </c>
+      <c r="AG32" s="72">
+        <v>4.6264000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E33" s="13" t="s">
         <v>11</v>
       </c>
@@ -10148,8 +11009,44 @@
       <c r="O33" s="16">
         <v>-25.9</v>
       </c>
-    </row>
-    <row r="34" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V33" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X33" s="71">
+        <v>-92.2</v>
+      </c>
+      <c r="Y33" s="71">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z33" s="71">
+        <v>16.2</v>
+      </c>
+      <c r="AA33" s="71">
+        <v>17.2</v>
+      </c>
+      <c r="AB33" s="71">
+        <v>15.1</v>
+      </c>
+      <c r="AC33" s="71">
+        <v>17</v>
+      </c>
+      <c r="AD33" s="71">
+        <v>15.1</v>
+      </c>
+      <c r="AE33" s="71">
+        <v>15.9</v>
+      </c>
+      <c r="AF33">
+        <v>3.4</v>
+      </c>
+      <c r="AG33" s="72">
+        <v>4.2835000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E34" s="13" t="s">
         <v>12</v>
       </c>
@@ -10180,8 +11077,44 @@
       <c r="O34" s="16">
         <v>-13.7</v>
       </c>
-    </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V34" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="X34" s="71">
+        <v>-95.1</v>
+      </c>
+      <c r="Y34" s="71">
+        <v>-0.5</v>
+      </c>
+      <c r="Z34" s="71">
+        <v>10</v>
+      </c>
+      <c r="AA34" s="71">
+        <v>10.5</v>
+      </c>
+      <c r="AB34" s="71">
+        <v>9.5</v>
+      </c>
+      <c r="AC34" s="71">
+        <v>10.1</v>
+      </c>
+      <c r="AD34" s="71">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AE34" s="71">
+        <v>9</v>
+      </c>
+      <c r="AF34">
+        <v>-1.8</v>
+      </c>
+      <c r="AG34" s="72">
+        <v>3.5867</v>
+      </c>
+    </row>
+    <row r="35" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E35" s="13" t="s">
         <v>13</v>
       </c>
@@ -10210,8 +11143,44 @@
       <c r="O35" s="16">
         <v>-6</v>
       </c>
-    </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V35" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="X35" s="71">
+        <v>-63.6</v>
+      </c>
+      <c r="Y35" s="71">
+        <v>30.6</v>
+      </c>
+      <c r="Z35" s="71">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="AA35" s="71">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="AB35" s="71">
+        <v>32.5</v>
+      </c>
+      <c r="AC35" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD35" s="71">
+        <v>25</v>
+      </c>
+      <c r="AE35" s="71">
+        <v>25.9</v>
+      </c>
+      <c r="AF35">
+        <v>5.4</v>
+      </c>
+      <c r="AG35" s="72">
+        <v>5.1485000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E36" s="13" t="s">
         <v>14</v>
       </c>
@@ -10242,8 +11211,44 @@
       <c r="O36" s="16">
         <v>-9.1999999999999993</v>
       </c>
-    </row>
-    <row r="37" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V36" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="X36" s="71">
+        <v>-82.9</v>
+      </c>
+      <c r="Y36" s="71">
+        <v>5.7</v>
+      </c>
+      <c r="Z36" s="71">
+        <v>14.2</v>
+      </c>
+      <c r="AA36" s="71">
+        <v>14.7</v>
+      </c>
+      <c r="AB36" s="71">
+        <v>13</v>
+      </c>
+      <c r="AC36" s="71">
+        <v>14.7</v>
+      </c>
+      <c r="AD36" s="71">
+        <v>12.9</v>
+      </c>
+      <c r="AE36" s="71">
+        <v>13.7</v>
+      </c>
+      <c r="AF36">
+        <v>3.5</v>
+      </c>
+      <c r="AG36" s="72">
+        <v>4.0979000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E37" s="14" t="s">
         <v>15</v>
       </c>
@@ -10274,8 +11279,44 @@
       <c r="O37" s="16">
         <v>-19.100000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="X37" s="71">
+        <v>-125</v>
+      </c>
+      <c r="Y37" s="71">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="71">
+        <v>11.4</v>
+      </c>
+      <c r="AA37" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB37" s="71">
+        <v>9.9</v>
+      </c>
+      <c r="AC37" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD37" s="71">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AE37" s="71">
+        <v>6</v>
+      </c>
+      <c r="AF37">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="AG37" s="72">
+        <v>3.7275</v>
+      </c>
+    </row>
+    <row r="38" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E38" s="13" t="s">
         <v>38</v>
       </c>
@@ -10306,8 +11347,44 @@
       <c r="O38" s="16">
         <v>-25.5</v>
       </c>
-    </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V38" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="X38" s="71">
+        <v>-82.7</v>
+      </c>
+      <c r="Y38" s="71">
+        <v>8.6</v>
+      </c>
+      <c r="Z38" s="71">
+        <v>16.3</v>
+      </c>
+      <c r="AA38" s="71">
+        <v>16.5</v>
+      </c>
+      <c r="AB38" s="71">
+        <v>15.2</v>
+      </c>
+      <c r="AC38" s="71">
+        <v>16.7</v>
+      </c>
+      <c r="AD38" s="71">
+        <v>9</v>
+      </c>
+      <c r="AE38" s="71">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AF38">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="AG38" s="72">
+        <v>3.6078000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="5:33" x14ac:dyDescent="0.2">
       <c r="F39" s="73" t="s">
         <v>74</v>
       </c>
@@ -10336,8 +11413,44 @@
         <f t="array" ref="O39">AVERAGE(ABS(O25:O38-$O25:$O38))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V39" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="X39" s="71">
+        <v>-80.7</v>
+      </c>
+      <c r="Y39" s="71">
+        <v>20.5</v>
+      </c>
+      <c r="Z39" s="71">
+        <v>26.3</v>
+      </c>
+      <c r="AA39" s="71">
+        <v>26.4</v>
+      </c>
+      <c r="AB39" s="71">
+        <v>25</v>
+      </c>
+      <c r="AC39" s="71">
+        <v>26.7</v>
+      </c>
+      <c r="AD39" s="71">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="AE39" s="71">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="AF39">
+        <v>1.7</v>
+      </c>
+      <c r="AG39" s="72">
+        <v>4.4058999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E40" s="13" t="s">
         <v>3</v>
       </c>
@@ -10354,8 +11467,44 @@
         <v>0.14705000000000013</v>
       </c>
       <c r="K40" s="23"/>
-    </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="V40" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="X40" s="71">
+        <v>-82.5</v>
+      </c>
+      <c r="Y40" s="71">
+        <v>20.9</v>
+      </c>
+      <c r="Z40" s="71">
+        <v>27.2</v>
+      </c>
+      <c r="AA40" s="71">
+        <v>27.4</v>
+      </c>
+      <c r="AB40" s="71">
+        <v>26.4</v>
+      </c>
+      <c r="AC40" s="71">
+        <v>27.7</v>
+      </c>
+      <c r="AD40" s="71">
+        <v>25.1</v>
+      </c>
+      <c r="AE40" s="71">
+        <v>25.5</v>
+      </c>
+      <c r="AF40">
+        <v>10</v>
+      </c>
+      <c r="AG40" s="72">
+        <v>5.0503999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E41" s="13" t="s">
         <v>4</v>
       </c>
@@ -10372,21 +11521,53 @@
         <v>-4.4109999999999983E-2</v>
       </c>
       <c r="K41" s="23"/>
-    </row>
-    <row r="42" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X41" s="40">
+        <f>ABS(X27-$AE27)</f>
+        <v>153.6</v>
+      </c>
+      <c r="Y41" s="40">
+        <f t="shared" ref="Y41:AE41" si="4">ABS(Y27-$AE27)</f>
+        <v>24.7</v>
+      </c>
+      <c r="Z41" s="40">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AA41" s="40">
+        <f t="shared" si="4"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="AB41" s="40">
+        <f t="shared" si="4"/>
+        <v>1.4999999999999996</v>
+      </c>
+      <c r="AC41" s="40">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AD41" s="40">
+        <f t="shared" si="4"/>
+        <v>1.4999999999999996</v>
+      </c>
+      <c r="AE41" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E42" s="14" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="23">
-        <f t="shared" ref="F42:H42" si="4">F27-$K7</f>
+        <f t="shared" ref="F42:H42" si="5">F27-$K7</f>
         <v>0.19999999999999929</v>
       </c>
       <c r="G42" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.5</v>
       </c>
       <c r="H42" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.9279200000000003</v>
       </c>
       <c r="J42" s="13" t="s">
@@ -10401,28 +11582,61 @@
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
       <c r="P42" s="23"/>
-    </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X42">
+        <f t="shared" ref="X42:AE54" si="6">ABS(X28-$AE28)</f>
+        <v>115.80000000000001</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="6"/>
+        <v>17.7</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="6"/>
+        <v>2.4</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="6"/>
+        <v>1.2</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="6"/>
+        <v>1.4</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF42" s="1"/>
+    </row>
+    <row r="43" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E43" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F43" s="23">
-        <f t="shared" ref="F43:H43" si="5">F28-$K8</f>
+        <f t="shared" ref="F43:H43" si="7">F28-$K8</f>
         <v>-2.8000000000000007</v>
       </c>
       <c r="G43" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-4.3000000000000007</v>
       </c>
       <c r="H43" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-4.5</v>
       </c>
       <c r="J43" s="13" t="s">
         <v>4</v>
       </c>
       <c r="K43" s="23">
-        <f t="shared" ref="K43:K55" si="6">L26-O26</f>
+        <f t="shared" ref="K43:K55" si="8">L26-O26</f>
         <v>-0.4</v>
       </c>
       <c r="L43" s="23"/>
@@ -10430,28 +11644,60 @@
       <c r="N43" s="23"/>
       <c r="O43" s="23"/>
       <c r="P43" s="23"/>
-    </row>
-    <row r="44" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X43">
+        <f t="shared" si="6"/>
+        <v>79.599999999999994</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="6"/>
+        <v>5.7999999999999989</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="AA43">
+        <f t="shared" si="6"/>
+        <v>1.7000000000000028</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="6"/>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="AC43">
+        <f t="shared" si="6"/>
+        <v>1.9000000000000021</v>
+      </c>
+      <c r="AD43">
+        <f t="shared" si="6"/>
+        <v>1.2999999999999972</v>
+      </c>
+      <c r="AE43">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E44" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="23">
-        <f t="shared" ref="F44:H44" si="7">F29-$K9</f>
+        <f t="shared" ref="F44:H44" si="9">F29-$K9</f>
         <v>0.5</v>
       </c>
       <c r="G44" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-0.40000000000000036</v>
       </c>
       <c r="H44" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-0.65596000000000032</v>
       </c>
       <c r="J44" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K44" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.5</v>
       </c>
       <c r="L44" s="23"/>
@@ -10459,28 +11705,60 @@
       <c r="N44" s="23"/>
       <c r="O44" s="23"/>
       <c r="P44" s="23"/>
-    </row>
-    <row r="45" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X44">
+        <f t="shared" si="6"/>
+        <v>101.69999999999999</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="6"/>
+        <v>6.6999999999999993</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="6"/>
+        <v>4.3000000000000007</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="6"/>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="AC44">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="AD44">
+        <f t="shared" si="6"/>
+        <v>1.1999999999999997</v>
+      </c>
+      <c r="AE44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E45" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="23">
-        <f t="shared" ref="F45:H45" si="8">F30-$K10</f>
+        <f t="shared" ref="F45:H45" si="10">F30-$K10</f>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="G45" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
       <c r="H45" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-0.60205999999999982</v>
       </c>
       <c r="J45" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K45" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-4.3000000000000007</v>
       </c>
       <c r="L45" s="23"/>
@@ -10488,28 +11766,60 @@
       <c r="N45" s="23"/>
       <c r="O45" s="23"/>
       <c r="P45" s="23"/>
-    </row>
-    <row r="46" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X45">
+        <f t="shared" si="6"/>
+        <v>94.8</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="6"/>
+        <v>8.2999999999999989</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="6"/>
+        <v>0.70000000000000107</v>
+      </c>
+      <c r="AB45">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="AC45">
+        <f t="shared" si="6"/>
+        <v>0.70000000000000107</v>
+      </c>
+      <c r="AD45">
+        <f t="shared" si="6"/>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="AE45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E46" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="23">
-        <f t="shared" ref="F46:H46" si="9">F31-$K11</f>
+        <f t="shared" ref="F46:H46" si="11">F31-$K11</f>
         <v>0.80000000000000071</v>
       </c>
       <c r="G46" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.29999999999999893</v>
       </c>
       <c r="H46" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.0603600000000011</v>
       </c>
       <c r="J46" s="13" t="s">
         <v>7</v>
       </c>
       <c r="K46" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.40000000000000036</v>
       </c>
       <c r="L46" s="23"/>
@@ -10517,28 +11827,60 @@
       <c r="N46" s="23"/>
       <c r="O46" s="23"/>
       <c r="P46" s="23"/>
-    </row>
-    <row r="47" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X46">
+        <f t="shared" si="6"/>
+        <v>99.4</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="6"/>
+        <v>10.9</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="6"/>
+        <v>1.2000000000000011</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="AC46">
+        <f t="shared" si="6"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="AD46">
+        <f t="shared" si="6"/>
+        <v>0.20000000000000107</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E47" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F47" s="23">
-        <f t="shared" ref="F47:H47" si="10">F32-$K12</f>
+        <f t="shared" ref="F47:H47" si="12">F32-$K12</f>
         <v>-0.5</v>
       </c>
       <c r="G47" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="H47" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.1168899999999997</v>
       </c>
       <c r="J47" s="14" t="s">
         <v>8</v>
       </c>
       <c r="K47" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.5</v>
       </c>
       <c r="L47" s="23"/>
@@ -10546,17 +11888,49 @@
       <c r="N47" s="23"/>
       <c r="O47" s="23"/>
       <c r="P47" s="23"/>
-    </row>
-    <row r="48" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X47">
+        <f t="shared" si="6"/>
+        <v>108.10000000000001</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="6"/>
+        <v>14.8</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="6"/>
+        <v>0.29999999999999893</v>
+      </c>
+      <c r="AA47">
+        <f t="shared" si="6"/>
+        <v>1.2999999999999989</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" si="6"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="AC47">
+        <f t="shared" si="6"/>
+        <v>1.0999999999999996</v>
+      </c>
+      <c r="AD47">
+        <f t="shared" si="6"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="AE47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="5:33" x14ac:dyDescent="0.2">
       <c r="E48" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F48" s="23">
-        <f t="shared" ref="F48:G48" si="11">F33-$K13</f>
+        <f t="shared" ref="F48:G48" si="13">F33-$K13</f>
         <v>-6.6000000000000014</v>
       </c>
       <c r="G48" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-8.8999999999999986</v>
       </c>
       <c r="H48" s="23"/>
@@ -10564,7 +11938,7 @@
         <v>9</v>
       </c>
       <c r="K48" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.29999999999999893</v>
       </c>
       <c r="L48" s="23"/>
@@ -10572,28 +11946,60 @@
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
       <c r="P48" s="23"/>
-    </row>
-    <row r="49" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X48">
+        <f t="shared" si="6"/>
+        <v>104.1</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="6"/>
+        <v>9.5</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AA48">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB48">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="AC48">
+        <f t="shared" si="6"/>
+        <v>1.0999999999999996</v>
+      </c>
+      <c r="AD48">
+        <f t="shared" si="6"/>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="AE48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:31" x14ac:dyDescent="0.2">
       <c r="E49" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F49" s="23">
-        <f t="shared" ref="F49:H49" si="12">F34-$K14</f>
+        <f t="shared" ref="F49:H49" si="14">F34-$K14</f>
         <v>0.69999999999999929</v>
       </c>
       <c r="G49" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.5</v>
       </c>
       <c r="H49" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-1.0037300000000009</v>
       </c>
       <c r="J49" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K49" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="L49" s="23"/>
@@ -10601,17 +12007,45 @@
       <c r="N49" s="23"/>
       <c r="O49" s="23"/>
       <c r="P49" s="23"/>
-    </row>
-    <row r="50" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X49">
+        <f t="shared" si="6"/>
+        <v>89.5</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="6"/>
+        <v>4.7000000000000028</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="6"/>
+        <v>8.8999999999999986</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="6"/>
+        <v>8.8999999999999986</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="6"/>
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="AD49">
+        <f t="shared" si="6"/>
+        <v>0.89999999999999858</v>
+      </c>
+      <c r="AE49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:31" x14ac:dyDescent="0.2">
       <c r="E50" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F50" s="23">
-        <f t="shared" ref="F50:G50" si="13">F35-$K15</f>
+        <f t="shared" ref="F50:G50" si="15">F35-$K15</f>
         <v>-3.9000000000000004</v>
       </c>
       <c r="G50" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-5.4</v>
       </c>
       <c r="H50" s="23"/>
@@ -10619,7 +12053,7 @@
         <v>11</v>
       </c>
       <c r="K50" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-8.8999999999999986</v>
       </c>
       <c r="L50" s="23"/>
@@ -10627,28 +12061,60 @@
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
       <c r="P50" s="23"/>
-    </row>
-    <row r="51" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X50">
+        <f t="shared" si="6"/>
+        <v>96.600000000000009</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="6"/>
+        <v>7.9999999999999991</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="AA50">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AB50">
+        <f t="shared" si="6"/>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="AC50">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AD50">
+        <f t="shared" si="6"/>
+        <v>0.79999999999999893</v>
+      </c>
+      <c r="AE50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="5:31" x14ac:dyDescent="0.2">
       <c r="E51" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F51" s="23">
-        <f t="shared" ref="F51:H51" si="14">F36-$K16</f>
+        <f t="shared" ref="F51:H51" si="16">F36-$K16</f>
         <v>-6</v>
       </c>
       <c r="G51" s="23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-7.1000000000000014</v>
       </c>
       <c r="H51" s="23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-7.5</v>
       </c>
       <c r="J51" s="13" t="s">
         <v>12</v>
       </c>
       <c r="K51" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.5</v>
       </c>
       <c r="L51" s="23"/>
@@ -10656,28 +12122,52 @@
       <c r="N51" s="23"/>
       <c r="O51" s="23"/>
       <c r="P51" s="23"/>
-    </row>
-    <row r="52" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X51">
+        <f t="shared" si="6"/>
+        <v>131</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" si="6"/>
+        <v>5.4</v>
+      </c>
+      <c r="AB51">
+        <f t="shared" si="6"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="AD51">
+        <f t="shared" si="6"/>
+        <v>0.90000000000000036</v>
+      </c>
+      <c r="AE51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:31" x14ac:dyDescent="0.2">
       <c r="E52" s="14" t="s">
         <v>15</v>
       </c>
       <c r="F52" s="23">
-        <f t="shared" ref="F52:H52" si="15">F37-$K17</f>
+        <f t="shared" ref="F52:H52" si="17">F37-$K17</f>
         <v>-5.8999999999999986</v>
       </c>
       <c r="G52" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>-7.1999999999999993</v>
       </c>
       <c r="H52" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>-7.5999999999999979</v>
       </c>
       <c r="J52" s="13" t="s">
         <v>13</v>
       </c>
       <c r="K52" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-5.4</v>
       </c>
       <c r="L52" s="23"/>
@@ -10685,28 +12175,60 @@
       <c r="N52" s="23"/>
       <c r="O52" s="23"/>
       <c r="P52" s="23"/>
-    </row>
-    <row r="53" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X52">
+        <f t="shared" si="6"/>
+        <v>91.9</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="6"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="6"/>
+        <v>7.1000000000000014</v>
+      </c>
+      <c r="AA52">
+        <f t="shared" si="6"/>
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="AB52">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AC52">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" si="6"/>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="AE52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="5:31" x14ac:dyDescent="0.2">
       <c r="E53" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F53" s="23">
-        <f t="shared" ref="F53:H53" si="16">F38-$K18</f>
+        <f t="shared" ref="F53:H53" si="18">F38-$K18</f>
         <v>-0.89999999999999858</v>
       </c>
       <c r="G53" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-1.6999999999999993</v>
       </c>
       <c r="H53" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-2.1999999999999993</v>
       </c>
       <c r="J53" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K53" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-7.1000000000000014</v>
       </c>
       <c r="L53" s="23"/>
@@ -10714,8 +12236,40 @@
       <c r="N53" s="23"/>
       <c r="O53" s="23"/>
       <c r="P53" s="23"/>
-    </row>
-    <row r="54" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X53">
+        <f t="shared" si="6"/>
+        <v>99.800000000000011</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" si="6"/>
+        <v>1.3999999999999986</v>
+      </c>
+      <c r="Z53">
+        <f t="shared" si="6"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="AA53">
+        <f t="shared" si="6"/>
+        <v>7.2999999999999972</v>
+      </c>
+      <c r="AB53">
+        <f t="shared" si="6"/>
+        <v>5.8999999999999986</v>
+      </c>
+      <c r="AC53">
+        <f t="shared" si="6"/>
+        <v>7.5999999999999979</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="AE53">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:31" x14ac:dyDescent="0.2">
       <c r="E54" s="53" t="s">
         <v>73</v>
       </c>
@@ -10735,7 +12289,7 @@
         <v>15</v>
       </c>
       <c r="K54" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-7.1999999999999993</v>
       </c>
       <c r="L54" s="23"/>
@@ -10743,13 +12297,45 @@
       <c r="N54" s="23"/>
       <c r="O54" s="23"/>
       <c r="P54" s="23"/>
-    </row>
-    <row r="55" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="X54" s="66">
+        <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+      <c r="Y54" s="66">
+        <f t="shared" si="6"/>
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="Z54" s="66">
+        <f t="shared" si="6"/>
+        <v>1.6999999999999993</v>
+      </c>
+      <c r="AA54" s="66">
+        <f t="shared" si="6"/>
+        <v>1.8999999999999986</v>
+      </c>
+      <c r="AB54" s="66">
+        <f t="shared" si="6"/>
+        <v>0.89999999999999858</v>
+      </c>
+      <c r="AC54" s="66">
+        <f t="shared" si="6"/>
+        <v>2.1999999999999993</v>
+      </c>
+      <c r="AD54" s="66">
+        <f t="shared" si="6"/>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="AE54" s="66">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="5:31" x14ac:dyDescent="0.2">
       <c r="J55" s="13" t="s">
         <v>38</v>
       </c>
       <c r="K55" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.6999999999999993</v>
       </c>
       <c r="L55" s="23"/>
@@ -10757,9 +12343,45 @@
       <c r="N55" s="23"/>
       <c r="O55" s="23"/>
       <c r="P55" s="23"/>
+      <c r="X55" s="23">
+        <f>AVERAGE(X41:X54)</f>
+        <v>105.27857142857144</v>
+      </c>
+      <c r="Y55" s="23">
+        <f t="shared" ref="Y55:AE55" si="19">AVERAGE(Y41:Y54)</f>
+        <v>8.7642857142857142</v>
+      </c>
+      <c r="Z55" s="23">
+        <f t="shared" si="19"/>
+        <v>2.8071428571428569</v>
+      </c>
+      <c r="AA55" s="23">
+        <f t="shared" si="19"/>
+        <v>3.3923076923076922</v>
+      </c>
+      <c r="AB55" s="23">
+        <f t="shared" si="19"/>
+        <v>2.2571428571428571</v>
+      </c>
+      <c r="AC55" s="23">
+        <f t="shared" si="19"/>
+        <v>2.3583333333333329</v>
+      </c>
+      <c r="AD55" s="23">
+        <f t="shared" si="19"/>
+        <v>0.76428571428571368</v>
+      </c>
+      <c r="AE55" s="23">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AD25:AE25"/>
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="K3:L3"/>
@@ -11968,23 +13590,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D977289-821A-854B-BFA8-F279ABC47434}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="81" t="s">
+      <c r="C1" s="85"/>
+      <c r="D1" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="82"/>
+      <c r="E1" s="84"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
       <c r="B2" s="50" t="s">
         <v>61</v>
       </c>
@@ -12203,59 +13828,163 @@
       <c r="E14" s="58"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
+      <c r="C15" s="86">
+        <v>1</v>
+      </c>
+      <c r="D15" s="59">
+        <v>2.02</v>
+      </c>
+      <c r="E15" s="59">
+        <v>1.54</v>
+      </c>
+      <c r="F15" s="49">
+        <v>1.64</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="86">
+        <v>2</v>
+      </c>
+      <c r="D16" s="59">
+        <v>1.95</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="47">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="86">
+        <v>3</v>
+      </c>
+      <c r="D17" s="59">
+        <v>1.89</v>
+      </c>
+      <c r="E17" s="59">
+        <v>1.39</v>
+      </c>
+      <c r="F17" s="47">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="86">
+        <v>4</v>
+      </c>
+      <c r="D18" s="59">
+        <v>1.89</v>
+      </c>
+      <c r="E18" s="59">
+        <v>1.4</v>
+      </c>
+      <c r="F18" s="47">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="86">
+        <v>5</v>
+      </c>
+      <c r="D19" s="59">
+        <v>1.84</v>
+      </c>
+      <c r="E19" s="59">
+        <v>1.34</v>
+      </c>
+      <c r="F19" s="47">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="86">
+        <v>6</v>
+      </c>
+      <c r="D20" s="59">
+        <v>1.83</v>
+      </c>
+      <c r="E20" s="59">
+        <v>1.32</v>
+      </c>
+      <c r="F20" s="47">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="86">
+        <v>7</v>
+      </c>
+      <c r="D21" s="59">
+        <v>1.65</v>
+      </c>
+      <c r="E21" s="59">
+        <v>1.17</v>
+      </c>
+      <c r="F21" s="47">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="86">
+        <v>8</v>
+      </c>
+      <c r="D22" s="59">
+        <v>1.88</v>
+      </c>
+      <c r="E22" s="59">
+        <v>1.39</v>
+      </c>
+      <c r="F22" s="47">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="86">
+        <v>9</v>
+      </c>
+      <c r="D23" s="59">
+        <v>1.97</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="47">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="86">
+        <v>10</v>
+      </c>
+      <c r="D24" s="59">
+        <v>1.92</v>
+      </c>
+      <c r="E24" s="59">
+        <v>1.45</v>
+      </c>
+      <c r="F24" s="47">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D25" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D26" s="58"/>
       <c r="E26" s="58"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D27" s="58"/>
       <c r="E27" s="58"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D28" s="58"/>
       <c r="E28" s="58"/>
     </row>
@@ -12265,6 +13994,7 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -13358,8 +15088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF798BE4-C0A1-7940-9885-95EEF6FDCBCD}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13986,12 +15716,12 @@
         <v>114473.92294368258</v>
       </c>
       <c r="K15">
-        <f>(K4-$J4)*27211.407953</f>
-        <v>-868.12198595148936</v>
+        <f t="shared" ref="K15:L15" si="7">(K4-K$13)*27211.407953</f>
+        <v>115313.83297725976</v>
       </c>
       <c r="L15">
-        <f>(L4-$J4)*27211.407953</f>
-        <v>-44.570961032540204</v>
+        <f t="shared" si="7"/>
+        <v>114441.69283780045</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -13999,16 +15729,16 @@
         <v>4</v>
       </c>
       <c r="J16">
-        <f>(J5-J$13)*27211.407953</f>
+        <f t="shared" ref="J16:L16" si="8">(J5-J$13)*27211.407953</f>
         <v>-9.7345138429135361</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:L16" si="7">(K5-$J5)*27211.407953</f>
-        <v>-2247.7368643387367</v>
+        <f t="shared" si="8"/>
+        <v>-549.43935865297476</v>
       </c>
       <c r="L16">
-        <f t="shared" si="7"/>
-        <v>-4.0408532618718986</v>
+        <f t="shared" si="8"/>
+        <v>-1.434511954378149</v>
       </c>
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.2">
@@ -14016,16 +15746,16 @@
         <v>6</v>
       </c>
       <c r="J17">
-        <f>(J6-J$13)*27211.407953</f>
+        <f t="shared" ref="J17:L17" si="9">(J6-J$13)*27211.407953</f>
         <v>-54.091655792522843</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:L17" si="8">(K6-$J6)*27211.407953</f>
-        <v>-1885.595008967693</v>
+        <f t="shared" si="9"/>
+        <v>-231.65464523154048</v>
       </c>
       <c r="L17">
-        <f t="shared" si="8"/>
-        <v>-39.719439108381621</v>
+        <f t="shared" si="9"/>
+        <v>-81.470239750497186</v>
       </c>
       <c r="M17" s="1"/>
     </row>
@@ -14034,16 +15764,16 @@
         <v>8</v>
       </c>
       <c r="J18">
-        <f>(J7-J$13)*27211.407953</f>
+        <f t="shared" ref="J18:L18" si="10">(J7-J$13)*27211.407953</f>
         <v>-5.6998430087997276</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:L18" si="9">(K7-$J7)*27211.407953</f>
-        <v>-1803.6648746535084</v>
+        <f t="shared" si="10"/>
+        <v>-101.33269813363262</v>
       </c>
       <c r="L18">
-        <f t="shared" si="9"/>
-        <v>-58.445706922394606</v>
+        <f t="shared" si="10"/>
+        <v>-51.804694780787045</v>
       </c>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.2">
@@ -14051,16 +15781,16 @@
         <v>10</v>
       </c>
       <c r="J19">
-        <f>(J8-J$13)*27211.407953</f>
+        <f t="shared" ref="J19:L19" si="11">(J8-J$13)*27211.407953</f>
         <v>2.8188295142117344E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K19:L19" si="10">(K8-$J8)*27211.407953</f>
-        <v>-1767.3356640433403</v>
+        <f t="shared" si="11"/>
+        <v>-59.275456219522859</v>
       </c>
       <c r="L19">
-        <f t="shared" si="10"/>
-        <v>-57.671841686850712</v>
+        <f t="shared" si="11"/>
+        <v>-45.302798241301311</v>
       </c>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.2">
@@ -14068,16 +15798,16 @@
         <v>12</v>
       </c>
       <c r="J20">
-        <f>(J9-J$13)*27211.407953</f>
+        <f t="shared" ref="J20:L20" si="12">(J9-J$13)*27211.407953</f>
         <v>0.78183817109653242</v>
       </c>
       <c r="K20">
-        <f t="shared" ref="K20:L20" si="11">(K9-$J9)*27211.407953</f>
-        <v>-1747.7720277381154</v>
+        <f t="shared" si="12"/>
+        <v>-38.958170038343347</v>
       </c>
       <c r="L20">
-        <f t="shared" si="11"/>
-        <v>-51.153890419404654</v>
+        <f t="shared" si="12"/>
+        <v>-38.031197097900836</v>
       </c>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.2">
@@ -14085,16 +15815,16 @@
         <v>15</v>
       </c>
       <c r="J21">
-        <f>(J10-J$13)*27211.407953</f>
+        <f t="shared" ref="J21:L21" si="13">(J10-J$13)*27211.407953</f>
         <v>0.66324813409682515</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:L21" si="12">(K10-$J10)*27211.407953</f>
-        <v>-1731.8827369631331</v>
+        <f t="shared" si="13"/>
+        <v>-23.187469300360863</v>
       </c>
       <c r="L21">
-        <f t="shared" si="12"/>
-        <v>-41.080442164357123</v>
+        <f t="shared" si="13"/>
+        <v>-28.076338879853015</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.2">
@@ -14102,16 +15832,16 @@
         <v>20</v>
       </c>
       <c r="J22">
-        <f>(J11-J$13)*27211.407953</f>
+        <f t="shared" ref="J22:L22" si="14">(J11-J$13)*27211.407953</f>
         <v>0.20742439853594022</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:L22" si="13">(K11-$J11)*27211.407953</f>
-        <v>-1719.6398537680323</v>
+        <f t="shared" si="14"/>
+        <v>-11.40040984082087</v>
       </c>
       <c r="L22">
-        <f t="shared" si="13"/>
-        <v>-29.280340281271553</v>
+        <f t="shared" si="14"/>
+        <v>-16.732060732328325</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.2">
@@ -14119,16 +15849,16 @@
         <v>30</v>
       </c>
       <c r="J23">
-        <f>(J12-J$13)*27211.407953</f>
+        <f t="shared" ref="J23:L23" si="15">(J12-J$13)*27211.407953</f>
         <v>6.9563242666231234E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23:L23" si="14">(K12-$J12)*27211.407953</f>
-        <v>-1711.0149667209166</v>
+        <f t="shared" si="15"/>
+        <v>-2.9133839495749703</v>
       </c>
       <c r="L23">
-        <f t="shared" si="14"/>
-        <v>-17.568942142633045</v>
+        <f t="shared" si="15"/>
+        <v>-5.1585237495595271</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.2">
@@ -14136,16 +15866,16 @@
         <v>40</v>
       </c>
       <c r="J24">
-        <f>(J13-J$13)*27211.407953</f>
+        <f t="shared" ref="J24:L24" si="16">(J13-J$13)*27211.407953</f>
         <v>0</v>
       </c>
       <c r="K24">
-        <f>(K13-$J13)*27.211407953</f>
-        <v>-1.7080320195286753</v>
+        <f t="shared" si="16"/>
+        <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="K24:L24" si="15">(L13-$J13)*27211.407953</f>
-        <v>-12.340855150407286</v>
+        <f t="shared" si="16"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.2">

</xml_diff>